<commit_message>
Changed values to match new data
</commit_message>
<xml_diff>
--- a/data/crossings_per_year_people.xlsx
+++ b/data/crossings_per_year_people.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrik/OneDrive/OOP2020/AI2020/jupyter/Bokeh/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrik/OneDrive/OOP2020/AI2020/Python-project/border-crossing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F909516-E831-2C4F-AAE4-B02F0766B617}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5BB484-AB57-5B4C-A895-CB1DD9CF5AC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5480" yWindow="2240" windowWidth="23320" windowHeight="13520" xr2:uid="{0AA7B50A-3372-2045-8FD9-921CB228C949}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440" xr2:uid="{5063F210-33E6-544A-9EE8-23CAA0FC387D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Blad1" sheetId="1" r:id="rId1"/>
+    <sheet name="Corrected data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,14 +38,14 @@
     <t>year</t>
   </si>
   <si>
-    <t>people_crossing_by_year</t>
+    <t>people</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -54,24 +54,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="15"/>
       <color theme="1"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1" tint="0.14999847407452621"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -86,13 +87,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -407,98 +411,100 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{833DC40B-C073-3A43-8431-727CA507B6DA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBE4B78B-D93D-8E41-A891-52BB14724507}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.39997558519241921"/>
+  </sheetPr>
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+    <row r="2" spans="1:2" ht="19" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
         <v>2011</v>
       </c>
       <c r="B2" s="2">
-        <v>330535715</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+        <v>153706850</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="19" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
         <v>2012</v>
       </c>
       <c r="B3" s="2">
-        <v>344503916</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+        <v>159061181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="19" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
         <v>2013</v>
       </c>
       <c r="B4" s="2">
-        <v>356218438</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+        <v>166151041</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="19" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
         <v>2014</v>
       </c>
       <c r="B5" s="2">
-        <v>364112233</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
+        <v>173260603</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="19" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
         <v>2015</v>
       </c>
       <c r="B6" s="2">
-        <v>365316686</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
+        <v>181281186</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="19" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
         <v>2016</v>
       </c>
       <c r="B7" s="2">
-        <v>367484183</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
+        <v>185155513</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="19" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
         <v>2017</v>
       </c>
       <c r="B8" s="2">
-        <v>372971276</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
+        <v>187965778</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="19" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
         <v>2018</v>
       </c>
       <c r="B9" s="2">
-        <v>379157530</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
+        <v>192913686</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="19" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
         <v>2019</v>
       </c>
       <c r="B10" s="2">
-        <v>370200249</v>
+        <v>188228921</v>
       </c>
     </row>
   </sheetData>

</xml_diff>